<commit_message>
Add remarks to grade form
</commit_message>
<xml_diff>
--- a/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
+++ b/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveadminwindesheim-my.sharepoint.com/personal/s1138990_student_windesheim_nl/Documents/Leerjaar 3/semester 2/Computer grapichs/homework 1/WebGL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Javascript\WebGL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{1B325467-ADB8-43B1-96C5-240180B61B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C279560D-1948-41A9-AE4E-03D741B22C9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792FCBCB-D4EB-4D6A-917A-AA59464BB460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -168,19 +168,28 @@
     <t>car, house, playground</t>
   </si>
   <si>
-    <t>Tree(spheres, cylinders), car, house, playground,plane</t>
-  </si>
-  <si>
-    <t>Spheres, cylinders, plane</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
-    <t>plane, tree leaves, tree log</t>
-  </si>
-  <si>
     <t>Color, side, map,  opacity, transparent</t>
+  </si>
+  <si>
+    <t>Orbit, flying and first person</t>
+  </si>
+  <si>
+    <t>Spheres, cylinders, plane, cone</t>
+  </si>
+  <si>
+    <t>comments, readable, multiple files, modular, multiple functions and a clear structure</t>
+  </si>
+  <si>
+    <t>Quaint little cabin in the woods with a moving car and a playground</t>
+  </si>
+  <si>
+    <t>Tree(spheres, cylinders), car, house, playground,plane and cone bush</t>
+  </si>
+  <si>
+    <t>plane, tree leaves, tree log, bush leaves</t>
   </si>
 </sst>
 </file>
@@ -667,7 +676,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -690,7 +699,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1015,8 +1024,8 @@
   </sheetPr>
   <dimension ref="B2:J37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1201,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="8"/>
       <c r="H22" s="27" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1202,7 +1211,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
       <c r="H23" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1222,7 +1231,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="9"/>
       <c r="H25" s="16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1232,7 +1241,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="9"/>
       <c r="H26" s="16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1252,7 +1261,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="9"/>
       <c r="H28" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1261,7 +1270,9 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="10"/>
-      <c r="H29" s="17"/>
+      <c r="H29" s="17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="11"/>
@@ -1302,7 +1313,9 @@
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="8"/>
-      <c r="H34" s="27"/>
+      <c r="H34" s="27" t="s">
+        <v>49</v>
+      </c>
       <c r="J34" s="28" t="s">
         <v>34</v>
       </c>
@@ -1313,7 +1326,9 @@
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="10"/>
-      <c r="H35" s="17"/>
+      <c r="H35" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="J35" s="15" t="s">
         <v>19</v>
       </c>
@@ -1348,20 +1363,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1611,28 +1618,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1658,9 +1663,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>